<commit_message>
Add modules Group Subject Student
</commit_message>
<xml_diff>
--- a/GradeReport.xlsx
+++ b/GradeReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\GradeReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1303103-153A-4799-8816-4452C6F09ACD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="3945" windowWidth="27555" windowHeight="14745" tabRatio="815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="3945" windowWidth="27555" windowHeight="14745" tabRatio="815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист5" sheetId="6" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="67">
   <si>
     <t>Матем</t>
   </si>
@@ -222,12 +221,18 @@
   </si>
   <si>
     <t>Не для всех выставленна</t>
+  </si>
+  <si>
+    <t>Закреплена на семестр</t>
+  </si>
+  <si>
+    <t>Закреплена на все где есть этот предмет</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -272,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -286,6 +291,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,7 +574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AD0C63-EACD-422D-A5B2-557000FA6CE6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист6"/>
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -718,11 +726,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA23595-18FE-4CF1-8811-4A122008E4D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,6 +908,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
@@ -948,11 +964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47476711-D290-499B-AB26-C66884B60C08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>